<commit_message>
se excluyen las carpetas temp
</commit_message>
<xml_diff>
--- a/temp_input_file/DATAMAPPING.xlsx
+++ b/temp_input_file/DATAMAPPING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Documents/EVERIS/Spring3/GoSpa/temp_input_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBB9122-3EFF-8F4E-87B5-3B5A3171D3FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C13E8A-725A-5245-B18E-64D4C7D78A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputMapping" sheetId="1" r:id="rId1"/>
@@ -17184,7 +17184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A4B5AD-1C38-4D20-8888-E675DC7A273B}">
   <dimension ref="A1:O345"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -32737,7 +32737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44FF62B-09F7-324E-BBEE-CE8CB1FE8493}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>